<commit_message>
Uploaded 10-May-2021 12:01:54 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3358" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3358" uniqueCount="329">
   <si>
     <t>RuleSet</t>
   </si>
@@ -1031,9 +1031,6 @@
   </si>
   <si>
     <t>tier4</t>
-  </si>
-  <si>
-    <t>$benefit1:Benefit</t>
   </si>
 </sst>
 </file>
@@ -1673,7 +1670,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>329</v>
+        <v>14</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 12:03:06 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -1667,10 +1667,10 @@
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>14</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 13:00:41 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -196,7 +196,7 @@
     <t>Declare</t>
   </si>
   <si>
-    <t>dialect java</t>
+    <t>dialect "java";</t>
   </si>
 </sst>
 </file>
@@ -788,7 +788,7 @@
   <dimension ref="A1:H1120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 14:07:13 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -1027,10 +1027,10 @@
     <t>getBenefit_group().getName()=="$param"</t>
   </si>
   <si>
-    <t>getName().equals=="$param"</t>
-  </si>
-  <si>
     <t>getHospitalTier()=="$param"</t>
+  </si>
+  <si>
+    <t>getName()=="$param"</t>
   </si>
 </sst>
 </file>
@@ -1607,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1687,10 +1687,10 @@
         <v>326</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>327</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>328</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 14:41:45 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -196,7 +196,7 @@
     <t>dialect "java";</t>
   </si>
   <si>
-    <t>getBenefit_group().getName()=="$param"</t>
+    <t>getBenefit_group().getName().equals("$param")</t>
   </si>
 </sst>
 </file>
@@ -788,7 +788,7 @@
   <dimension ref="A1:H1120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 14:48:23 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -196,7 +196,7 @@
     <t>dialect "java";</t>
   </si>
   <si>
-    <t>getBenefit_group().getName().equals("$param")</t>
+    <t>getBenefit_group().getName()==$param</t>
   </si>
 </sst>
 </file>
@@ -787,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 15:23:56 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -196,7 +196,7 @@
     <t>dialect "java";</t>
   </si>
   <si>
-    <t>name=="$param"</t>
+    <t>benefit_group.name.equals("$param")</t>
   </si>
 </sst>
 </file>
@@ -787,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 16:04:03 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -196,7 +196,7 @@
     <t>dialect "java";</t>
   </si>
   <si>
-    <t>benefit_group.name=="aa"</t>
+    <t>benefit_group.name</t>
   </si>
 </sst>
 </file>
@@ -788,7 +788,7 @@
   <dimension ref="A1:H1120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 16:43:59 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -187,7 +187,7 @@
     <t>$benefit : Benefit</t>
   </si>
   <si>
-    <t>getBenefit_group().getName()=="$param"</t>
+    <t>getBenefit_group().getName().equals("$param")</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,7 @@
   <dimension ref="A1:H1118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Uploaded 10-May-2021 17:03:31 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -167,9 +167,6 @@
     <t>Declare</t>
   </si>
   <si>
-    <t>getBenefit_group().getName().equals("$param")</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">RuleTable </t>
     </r>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>dialect "java"</t>
+  </si>
+  <si>
+    <t>(getBenefit_group().getName()).equals("$param")</t>
   </si>
 </sst>
 </file>
@@ -783,7 +783,7 @@
   <dimension ref="A1:H1119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -813,14 +813,14 @@
         <v>46</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -855,7 +855,7 @@
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Uploaded 11-May-2021 11:00:07 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3356" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3357" uniqueCount="329">
   <si>
     <t>RuleSet</t>
   </si>
@@ -1213,6 +1213,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1220,12 +1226,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1603,7 +1603,7 @@
   <dimension ref="A1:J1118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1624,23 +1624,23 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1650,10 +1650,12 @@
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="23"/>
+      <c r="D3" s="20" t="s">
+        <v>5</v>
+      </c>
       <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
@@ -1665,10 +1667,10 @@
     <row r="4" spans="1:10" ht="25.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="22" t="s">
         <v>325</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
@@ -25064,11 +25066,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Uploaded 11-May-2021 11:08:17 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -1213,6 +1213,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1221,12 +1227,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1603,7 +1603,7 @@
   <dimension ref="A1:J1118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1624,23 +1624,23 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1650,10 +1650,10 @@
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="22" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -1667,10 +1667,10 @@
     <row r="4" spans="1:10" ht="25.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="D4" s="23"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
@@ -25066,10 +25066,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Uploaded 12-May-2021 09:44:24 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>RuleSet</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t>$benefit.setCalculationResult($param);</t>
+  </si>
+  <si>
+    <t>GENERAL CONSULTATION</t>
+  </si>
+  <si>
+    <t>Basic outpatient and in-patient Treatment</t>
+  </si>
+  <si>
+    <t>tier1</t>
+  </si>
+  <si>
+    <t>TariffDecision1</t>
   </si>
 </sst>
 </file>
@@ -192,7 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -226,6 +238,15 @@
     </xf>
     <xf numFmtId="10" fontId="5" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -529,13 +550,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -605,6 +633,26 @@
       </c>
       <c r="F5" s="10" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="13">
+        <v>20</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="14">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded 12-May-2021 09:49:09 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>RuleSet</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>TariffDecision1</t>
+  </si>
+  <si>
+    <t>TariffDecision2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECIALIST CONSULTATION </t>
+  </si>
+  <si>
+    <t>Obstetrician</t>
   </si>
 </sst>
 </file>
@@ -204,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -218,35 +227,44 @@
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="5" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -550,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,23 +588,23 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -609,30 +627,30 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -640,20 +658,40 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="10">
         <v>20</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="11">
         <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="13">
+        <v>20</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="14">
+        <v>150000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded 12-May-2021 09:51:43 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>RuleSet</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Obstetrician</t>
+  </si>
+  <si>
+    <t>Gynaecologist</t>
+  </si>
+  <si>
+    <t>Pediatrician</t>
+  </si>
+  <si>
+    <t>TariffDecision3</t>
+  </si>
+  <si>
+    <t>TariffDecision4</t>
   </si>
 </sst>
 </file>
@@ -213,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -239,24 +251,6 @@
     <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -265,6 +259,15 @@
     </xf>
     <xf numFmtId="10" fontId="5" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -568,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,23 +591,23 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -629,16 +632,16 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
@@ -654,37 +657,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="12">
         <v>20</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="14">
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>20</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="14" t="s">
@@ -692,6 +695,46 @@
       </c>
       <c r="F7" s="14">
         <v>150000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="12">
+        <v>20</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="14">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="12">
+        <v>20</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="14">
+        <v>15000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded 12-May-2021 09:52:48 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>RuleSet</t>
   </si>
@@ -69,16 +69,7 @@
     <t>$benefit.setCalculationResult($param);</t>
   </si>
   <si>
-    <t>GENERAL CONSULTATION</t>
-  </si>
-  <si>
-    <t>Basic outpatient and in-patient Treatment</t>
-  </si>
-  <si>
     <t>tier1</t>
-  </si>
-  <si>
-    <t>TariffDecision1</t>
   </si>
   <si>
     <t>TariffDecision2</t>
@@ -571,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,41 +648,41 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="12">
         <v>20</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>15</v>
-      </c>
       <c r="F6" s="14">
-        <v>2000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="12">
         <v>20</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7" s="14">
         <v>150000</v>
@@ -699,41 +690,21 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="12">
         <v>20</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>20</v>
-      </c>
       <c r="E8" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" s="14">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="12">
-        <v>20</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="14">
         <v>15000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 12-May-2021 09:54:22 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>RuleSet</t>
   </si>
@@ -72,15 +72,9 @@
     <t>tier1</t>
   </si>
   <si>
-    <t>TariffDecision2</t>
-  </si>
-  <si>
     <t xml:space="preserve">SPECIALIST CONSULTATION </t>
   </si>
   <si>
-    <t>Obstetrician</t>
-  </si>
-  <si>
     <t>Gynaecologist</t>
   </si>
   <si>
@@ -91,13 +85,25 @@
   </si>
   <si>
     <t>TariffDecision4</t>
+  </si>
+  <si>
+    <t>Benefit group</t>
+  </si>
+  <si>
+    <t>Benefit</t>
+  </si>
+  <si>
+    <t>HospitalTier</t>
+  </si>
+  <si>
+    <t>CalculationResult</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,8 +147,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +175,12 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -216,7 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -259,6 +279,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -564,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,38 +677,38 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="12">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="14">
-        <v>150000</v>
+      <c r="E6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="12">
         <v>20</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>17</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>13</v>
@@ -690,16 +719,16 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="12">
         <v>20</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Uploaded 12-May-2021 10:00:00 {/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/TariffDecision.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>RuleSet</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>Pediatrician</t>
-  </si>
-  <si>
-    <t>TariffDecision3</t>
-  </si>
-  <si>
-    <t>TariffDecision4</t>
   </si>
   <si>
     <t>Benefit group</t>
@@ -594,12 +588,12 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="29.140625" customWidth="1"/>
@@ -685,21 +679,22 @@
         <v>4</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="F6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="str">
+        <f>CONCATENATE("Tariff ",C7,D7,"-",E7)</f>
+        <v>Tariff SPECIALIST CONSULTATION Gynaecologist-tier1</v>
       </c>
       <c r="B7" s="12">
         <v>20</v>
@@ -717,9 +712,10 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="str">
+        <f>CONCATENATE("Tariff ",C8,D8,"-",E8)</f>
+        <v>Tariff SPECIALIST CONSULTATION Pediatrician-tier1</v>
       </c>
       <c r="B8" s="12">
         <v>20</v>

</xml_diff>